<commit_message>
Actualizar: Fase2.ipynb, Fase3_1.xlsx, HR_CLEAN_DATA.csv
</commit_message>
<xml_diff>
--- a/Fase3_1.xlsx
+++ b/Fase3_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34679\OneDrive\Documentos\ADALAB\Modulo3\Repos\project-da-promo-H-module-3-team-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3294B98-7C9D-4D6F-9E92-73A92024FF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08259B11-9BE5-4386-8D0D-354BBF03B7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11748" yWindow="0" windowWidth="11412" windowHeight="11892" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="129">
   <si>
     <t>NOMBRE COLUMNA ORIGINAL</t>
   </si>
@@ -455,14 +455,17 @@
     <t xml:space="preserve">Faltan valores. Identificar los números que faltan y utilizarlos para terminar de rellenar la columna. </t>
   </si>
   <si>
-    <t>Muchos nulos, a espera de clase de nulos.</t>
+    <t>Muchos nulos, ELIMINAMOS</t>
+  </si>
+  <si>
+    <t>Demasiados nulos. ¿Borrar?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -491,8 +494,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +550,24 @@
         <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -554,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -595,6 +622,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,10 +1020,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1121,21 +1162,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="J8" t="s">
-        <v>32</v>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="J8" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -1535,17 +1579,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="36" spans="2:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="D36" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="J36" s="23" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizar: Fase2.ipynb, Fase3_1.xlsx y HR_CLEAN_DATA.csv
</commit_message>
<xml_diff>
--- a/Fase3_1.xlsx
+++ b/Fase3_1.xlsx
@@ -12,7 +12,7 @@
     <sheet name="COL_ELIMINADAS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">BBDD!$B$1:$K$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">BBDD!$B$1:$K$36</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="138">
   <si>
     <t xml:space="preserve">NOMBRE COLUMNA ORIGINAL</t>
   </si>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">object</t>
   </si>
   <si>
-    <t xml:space="preserve">Añadir columna</t>
+    <t xml:space="preserve">Añadir columna y Añadir valores</t>
   </si>
   <si>
     <t xml:space="preserve">Attrition</t>
@@ -92,7 +92,32 @@
     <t xml:space="preserve">Business_Travel</t>
   </si>
   <si>
-    <t xml:space="preserve">[nan, 'travel_rarely', 'travel_frequently', 'non-travel']</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'Unknown'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, 'Travel Rarely', 'Travel Frequently', 'Non Travel']</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eliminar guiones y cambiar a .title()</t>
@@ -116,7 +141,7 @@
     <t xml:space="preserve">Department</t>
   </si>
   <si>
-    <t xml:space="preserve">['Unknow', ' Research &amp; Development ', ' Sales ', ' Human Resources ']</t>
+    <t xml:space="preserve">['Unknown', 'Research &amp; Development', 'Sales', 'Human Resources']</t>
   </si>
   <si>
     <t xml:space="preserve">Rellenar nulos con columna 'Job Role'</t>
@@ -146,8 +171,33 @@
     <t xml:space="preserve">Education_Field</t>
   </si>
   <si>
-    <t xml:space="preserve">[nan, 'Life Sciences', 'Technical Degree', 'Medical', 'Other',
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'Unknown'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, 'Life Sciences', 'Technical Degree', 'Medical', 'Other',
        'Marketing', 'Human Resources']</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Cambiar a .title()</t>
@@ -168,6 +218,9 @@
     <t xml:space="preserve">Faltan valores.</t>
   </si>
   <si>
+    <t xml:space="preserve">Reemplazar NaN con nuevos numeros</t>
+  </si>
+  <si>
     <t xml:space="preserve">EnvironmentSatisfaction</t>
   </si>
   <si>
@@ -196,6 +249,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cambiar 'Not Available' /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reemplazar NaN por 99999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job_Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Añadir columna con Job_Role + Department (MH, MS..)</t>
   </si>
   <si>
     <t xml:space="preserve">JobInvolvement</t>
@@ -309,6 +371,9 @@
     <t xml:space="preserve">valor &lt;= 100</t>
   </si>
   <si>
+    <t xml:space="preserve">cambiar a 0.25?</t>
+  </si>
+  <si>
     <t xml:space="preserve">PerformanceRating</t>
   </si>
   <si>
@@ -460,7 +525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -491,6 +556,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -512,6 +582,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
       </patternFill>
@@ -520,12 +596,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -597,7 +667,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -674,19 +744,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,43 +772,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,11 +824,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -839,15 +913,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K39"/>
+  <dimension ref="B1:K40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+      <selection pane="bottomLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.52"/>
@@ -925,7 +999,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="19" t="s">
         <v>16</v>
       </c>
       <c r="K3" s="17"/>
@@ -940,7 +1014,7 @@
       <c r="D4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="20" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="15"/>
@@ -959,7 +1033,7 @@
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="21" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="15"/>
@@ -979,7 +1053,7 @@
       <c r="C6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="22" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="14"/>
@@ -1001,13 +1075,13 @@
       <c r="D7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="21" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="23" t="s">
         <v>31</v>
       </c>
       <c r="K7" s="17" t="s">
@@ -1052,7 +1126,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" s="11" customFormat="true" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="11" customFormat="true" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12" t="s">
         <v>38</v>
       </c>
@@ -1062,7 +1136,7 @@
       <c r="D10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="15"/>
@@ -1079,7 +1153,7 @@
       <c r="B11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -1097,56 +1171,58 @@
       <c r="J11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="17"/>
+      <c r="K11" s="17" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>49</v>
+      <c r="E12" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="J12" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K12" s="17"/>
     </row>
     <row r="13" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>52</v>
+      <c r="E13" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="J13" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K13" s="17"/>
     </row>
     <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22" t="s">
-        <v>54</v>
+      <c r="B14" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>11</v>
@@ -1155,135 +1231,135 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="J14" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="24"/>
-    </row>
-    <row r="15" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="J14" s="25" t="s">
         <v>57</v>
       </c>
+      <c r="K14" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" s="11" customFormat="true" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="24" t="s">
+        <v>13</v>
+      </c>
       <c r="C15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>37</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="17"/>
+      <c r="J15" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="J16" s="23"/>
+      <c r="J16" s="25"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
-      <c r="J17" s="16" t="s">
-        <v>63</v>
-      </c>
+      <c r="J17" s="25"/>
       <c r="K17" s="17"/>
     </row>
     <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>37</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E18" s="14"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="J18" s="23"/>
+      <c r="J18" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="K18" s="17"/>
     </row>
     <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="J19" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="K19" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="25"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="27" t="s">
         <v>71</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="14"/>
+        <v>15</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="22" t="s">
+      <c r="J20" s="16" t="s">
         <v>73</v>
       </c>
+      <c r="K20" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="C21" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>11</v>
@@ -1292,48 +1368,46 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="J21" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="K21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="29" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
-        <v>76</v>
+      <c r="B22" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="J22" s="23"/>
+      <c r="J22" s="25" t="s">
+        <v>79</v>
+      </c>
       <c r="K22" s="17"/>
     </row>
     <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>80</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E23" s="14"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="23" t="s">
-        <v>81</v>
-      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="12" t="s">
@@ -1343,103 +1417,105 @@
         <v>83</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>84</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="25" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>37</v>
+      <c r="E25" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="23" t="s">
-        <v>87</v>
-      </c>
+      <c r="J25" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="K25" s="17"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="25" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>92</v>
+      <c r="E27" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="J27" s="23"/>
+      <c r="J27" s="25"/>
       <c r="K27" s="17"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="14"/>
+      <c r="E28" s="20" t="s">
+        <v>97</v>
+      </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="J28" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="K28" s="26" t="s">
-        <v>96</v>
-      </c>
+      <c r="J28" s="25"/>
+      <c r="K28" s="17"/>
     </row>
     <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>34</v>
@@ -1448,55 +1524,59 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="17"/>
+      <c r="J29" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="E30" s="14"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="J30" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="K30" s="26" t="s">
-        <v>101</v>
-      </c>
+      <c r="J30" s="25"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="17"/>
+      <c r="J31" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>34</v>
@@ -1505,17 +1585,15 @@
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="J32" s="16" t="s">
-        <v>106</v>
-      </c>
+      <c r="J32" s="25"/>
       <c r="K32" s="17"/>
     </row>
     <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>34</v>
@@ -1525,16 +1603,16 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="J33" s="16" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="K33" s="17"/>
     </row>
     <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="12" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>34</v>
@@ -1550,32 +1628,40 @@
     </row>
     <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>19</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E35" s="14"/>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="J35" s="16"/>
+      <c r="J35" s="16" t="s">
+        <v>116</v>
+      </c>
       <c r="K35" s="17"/>
     </row>
     <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
-      <c r="J36" s="23"/>
+      <c r="J36" s="16"/>
       <c r="K36" s="17"/>
     </row>
     <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1672,7 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
-      <c r="J37" s="23"/>
+      <c r="J37" s="25"/>
       <c r="K37" s="17"/>
     </row>
     <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,24 +1683,35 @@
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
-      <c r="J38" s="23"/>
+      <c r="J38" s="25"/>
       <c r="K38" s="17"/>
     </row>
-    <row r="39" s="29" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="33"/>
+    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="17"/>
+    </row>
+    <row r="40" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="31"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="34"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K35"/>
+  <autoFilter ref="B1:K36"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1637,7 +1734,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.63"/>
@@ -1646,185 +1743,185 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="35" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
       <c r="J2" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="J3" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
       <c r="J4" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="J5" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="J5" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
       <c r="J6" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
       <c r="J7" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
-      <c r="J8" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>128</v>
+      <c r="J8" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
       <c r="J9" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
       <c r="J10" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar Fase2 y Fase3_1
</commit_message>
<xml_diff>
--- a/Fase3_1.xlsx
+++ b/Fase3_1.xlsx
@@ -12,7 +12,7 @@
     <sheet name="COL_ELIMINADAS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">BBDD!$B$1:$K$36</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">BBDD!$B$1:$K$35</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -239,7 +239,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cambiar 'Marr</t>
     </r>
@@ -249,7 +248,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ei</t>
     </r>
@@ -258,12 +256,164 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">d' por 'Married'. Cambiar todo a .title()</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">MonthlyRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly_Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cómo relacionar con monthly income?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMCOMPANIESWORKED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num_Companies_Worked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OverTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over_Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[True, False, Unknown]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reemplazar NaN por 'Unknown'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PercentSalaryHike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent_Salary_Hike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor &lt;= 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cambiar a 0.25?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PerformanceRating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance_Rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reemlazar nan por median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RelationshipSatisfaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relationship_Satisfaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satisfaction_Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['A','B']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear columna y grupos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StockOptionLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock_Option_Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0, 1, 2, 3,4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTALWORKINGYEARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total_Working_Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar ',0'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reemplazar NaN con median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrainingTimesLastYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training_Times_Last_Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKLIFEBALANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work_Life_Balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YearsAtCompany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years_At_Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YearsSinceLastPromotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years_Since_Last_Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ninguna es mayor que tears at company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YEARSWITHCURRMANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years_With_Curr_Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DateBirth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date_Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los datos coinciden con 'Over18'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RemoteWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote_Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enviromentsatisfaction/jobsatisfaction/ relationshipSatisfaction --&gt; Son todas diferentes e importantes?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index_col</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELIMINAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employeecount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee_Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int64</t>
+  </si>
+  <si>
     <t xml:space="preserve">MonthlyIncome</t>
   </si>
   <si>
@@ -271,159 +421,6 @@
   </si>
   <si>
     <t xml:space="preserve">Reemplazar Nan con Use KNNImputer or IterativeImputer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MonthlyRate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly_Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cómo relacionar con monthly income?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMCOMPANIESWORKED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Num_Companies_Worked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OverTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Over_Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[True, False, Unknown]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reemplazar NaN por 'Unknown'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PercentSalaryHike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent_Salary_Hike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valor &lt;= 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cambiar a 0.25?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PerformanceRating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance_Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reemlazar nan por median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RelationshipSatisfaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relationship_Satisfaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Satisfaction_Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['A','B']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crear columna y grupos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StockOptionLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock_Option_Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0, 1, 2, 3] cambiar a [1,2,3,4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTALWORKINGYEARS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total_Working_Years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar ',0'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reemplazar NaN con median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrainingTimesLastYear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training_Times_Last_Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORKLIFEBALANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work_Life_Balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YearsAtCompany</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years_At_Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YearsSinceLastPromotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years_Since_Last_Promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ninguna es mayor que tears at company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YEARSWITHCURRMANAGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years_With_Curr_Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DateBirth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date_Birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los datos coinciden con 'Over18'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RemoteWork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remote_Work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enviromentsatisfaction/jobsatisfaction/ relationshipSatisfaction --&gt; Son todas diferentes e importantes?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index_col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELIMINAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employeecount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee_Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int64</t>
   </si>
   <si>
     <t xml:space="preserve">Over18</t>
@@ -480,7 +477,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -502,17 +498,15 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,7 +516,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FF99"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF66FF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor rgb="FF66FF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -533,14 +539,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -551,8 +551,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -705,7 +705,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -713,51 +717,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -766,6 +758,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -826,7 +826,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF66FF99"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF66FF66"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF6600"/>
@@ -854,15 +854,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K40"/>
+  <dimension ref="B1:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.52"/>
@@ -872,7 +872,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="33.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="33.22"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +964,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="17"/>
     </row>
-    <row r="5" s="11" customFormat="true" ht="25.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="12" t="s">
         <v>20</v>
       </c>
@@ -987,7 +987,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" s="11" customFormat="true" ht="25.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="11" customFormat="true" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="12" t="s">
         <v>25</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="19" t="s">
         <v>31</v>
       </c>
       <c r="K7" s="21" t="s">
@@ -1069,7 +1069,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" s="11" customFormat="true" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="11" customFormat="true" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12" t="s">
         <v>37</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="B11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="11" customFormat="true" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="12" t="s">
         <v>51</v>
       </c>
@@ -1160,8 +1160,8 @@
       </c>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="24" t="s">
+    <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -1174,7 +1174,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="24" t="s">
         <v>56</v>
       </c>
       <c r="K14" s="22" t="s">
@@ -1197,7 +1197,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="J15" s="25"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="17"/>
     </row>
     <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,7 +1216,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="J16" s="25"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,14 +1254,14 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="J18" s="25"/>
+      <c r="J18" s="24"/>
       <c r="K18" s="17"/>
     </row>
     <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>67</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -1280,8 +1280,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12" t="s">
+    <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="23" t="s">
         <v>70</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -1294,13 +1294,13 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="27" t="s">
+      <c r="J20" s="24" t="s">
         <v>72</v>
       </c>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="12" t="s">
         <v>73</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -1313,69 +1313,71 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="J21" s="25" t="s">
-        <v>75</v>
-      </c>
+      <c r="J21" s="24"/>
       <c r="K21" s="17"/>
     </row>
     <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="D22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="14"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="16" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="J23" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="17"/>
+      <c r="K24" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="K24" s="17"/>
     </row>
     <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="12" t="s">
@@ -1393,50 +1395,48 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="16" t="s">
+      <c r="J25" s="24"/>
+      <c r="K25" s="17"/>
+    </row>
+    <row r="26" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12" t="s">
+      <c r="D26" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="J26" s="25"/>
+      <c r="J26" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="K26" s="17"/>
     </row>
     <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="12"/>
+      <c r="B27" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="C27" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="J27" s="25" t="s">
-        <v>94</v>
-      </c>
+      <c r="J27" s="24"/>
       <c r="K27" s="17"/>
     </row>
-    <row r="28" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="12" t="s">
         <v>95</v>
       </c>
@@ -1446,21 +1446,23 @@
       <c r="D28" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>97</v>
-      </c>
+      <c r="E28" s="14"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="17"/>
-    </row>
-    <row r="29" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K28" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>11</v>
@@ -1469,59 +1471,55 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="J29" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>101</v>
-      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="17"/>
     </row>
     <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>103</v>
-      </c>
       <c r="D30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="14"/>
+      <c r="E30" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="17"/>
-    </row>
-    <row r="31" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K30" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="D31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="20" t="s">
-        <v>36</v>
-      </c>
+      <c r="E31" s="14"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
-      <c r="J31" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="K31" s="21" t="s">
-        <v>101</v>
-      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="17"/>
     </row>
     <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>11</v>
@@ -1530,10 +1528,12 @@
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="J32" s="25"/>
+      <c r="J32" s="16" t="s">
+        <v>107</v>
+      </c>
       <c r="K32" s="17"/>
     </row>
-    <row r="33" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="12" t="s">
         <v>108</v>
       </c>
@@ -1548,16 +1548,16 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="J33" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K33" s="17"/>
+    </row>
+    <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="K33" s="17"/>
-    </row>
-    <row r="34" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>11</v>
@@ -1567,11 +1567,11 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="J34" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K34" s="17"/>
     </row>
-    <row r="35" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="12" t="s">
         <v>113</v>
       </c>
@@ -1579,34 +1579,26 @@
         <v>114</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="14"/>
+        <v>18</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="J35" s="16" t="s">
-        <v>115</v>
-      </c>
+      <c r="J35" s="16"/>
       <c r="K35" s="17"/>
     </row>
     <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="14"/>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
-      <c r="J36" s="16"/>
+      <c r="J36" s="24"/>
       <c r="K36" s="17"/>
     </row>
     <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,7 +1609,7 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
-      <c r="J37" s="25"/>
+      <c r="J37" s="24"/>
       <c r="K37" s="17"/>
     </row>
     <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,35 +1620,24 @@
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
-      <c r="J38" s="25"/>
+      <c r="J38" s="24"/>
       <c r="K38" s="17"/>
     </row>
-    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="17"/>
-    </row>
-    <row r="40" s="29" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="33"/>
+    <row r="39" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K36"/>
+  <autoFilter ref="B1:K35"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1673,13 +1654,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K10"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.63"/>
@@ -1687,186 +1668,205 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="34" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="J2" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="J3" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" s="11" customFormat="true" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="37" t="s">
         <v>123</v>
-      </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="J3" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="J4" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+        <v>125</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
       <c r="J5" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
       <c r="J6" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="J7" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="J7" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="J8" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="J8" s="25" t="s">
+      <c r="D9" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="J9" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K9" s="39" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="J9" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="J10" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="J10" s="0" t="s">
+      <c r="D11" s="35" t="s">
         <v>120</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="J11" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>